<commit_message>
hide create data, add truncate to title product
</commit_message>
<xml_diff>
--- a/app/assets/data_product.xlsx
+++ b/app/assets/data_product.xlsx
@@ -1454,13 +1454,10 @@
   <dimension ref="A1:H143"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A122" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G124" activeCellId="0" sqref="G124"/>
+      <selection pane="topLeft" activeCell="G124" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4033,7 +4030,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="237.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>7854</v>
       </c>

</xml_diff>